<commit_message>
Añadido random forest regressor y graficas
</commit_message>
<xml_diff>
--- a/dr_EES_2018.xlsx
+++ b/dr_EES_2018.xlsx
@@ -1382,9 +1382,6 @@
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1395,15 +1392,18 @@
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4936,7 +4936,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
+      <selection pane="bottomLeft" activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5407,7 +5407,7 @@
       <c r="J16" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="K16" s="72" t="s">
+      <c r="K16" s="79" t="s">
         <v>291</v>
       </c>
     </row>
@@ -5438,7 +5438,7 @@
       <c r="J17" s="24" t="s">
         <v>275</v>
       </c>
-      <c r="K17" s="72"/>
+      <c r="K17" s="79"/>
     </row>
     <row r="18" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="67" t="s">
@@ -5695,7 +5695,7 @@
       <c r="J26" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="K26" s="72" t="s">
+      <c r="K26" s="79" t="s">
         <v>292</v>
       </c>
     </row>
@@ -5726,7 +5726,7 @@
       <c r="J27" s="24" t="s">
         <v>279</v>
       </c>
-      <c r="K27" s="72"/>
+      <c r="K27" s="79"/>
     </row>
     <row r="28" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="67" t="s">
@@ -5785,31 +5785,31 @@
       </c>
     </row>
     <row r="30" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="73" t="s">
+      <c r="A30" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="74" t="s">
+      <c r="B30" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="C30" s="75">
-        <v>1</v>
-      </c>
-      <c r="D30" s="75" t="s">
+      <c r="C30" s="74">
+        <v>1</v>
+      </c>
+      <c r="D30" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75">
+      <c r="E30" s="74"/>
+      <c r="F30" s="74">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="G30" s="75">
+      <c r="G30" s="74">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="H30" s="76" t="s">
+      <c r="H30" s="75" t="s">
         <v>285</v>
       </c>
-      <c r="I30" s="74" t="s">
+      <c r="I30" s="73" t="s">
         <v>80</v>
       </c>
       <c r="J30" s="24"/>
@@ -5818,27 +5818,27 @@
       </c>
     </row>
     <row r="31" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="73" t="s">
+      <c r="A31" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="74"/>
-      <c r="C31" s="75">
+      <c r="B31" s="73"/>
+      <c r="C31" s="74">
         <v>2</v>
       </c>
-      <c r="D31" s="75" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75">
+      <c r="D31" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="G31" s="75">
+      <c r="G31" s="74">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="H31" s="75"/>
-      <c r="I31" s="74" t="s">
+      <c r="H31" s="74"/>
+      <c r="I31" s="73" t="s">
         <v>81</v>
       </c>
       <c r="J31" s="24" t="s">
@@ -5846,31 +5846,31 @@
       </c>
     </row>
     <row r="32" spans="1:11" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="73" t="s">
+      <c r="A32" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="74" t="s">
+      <c r="B32" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="75">
-        <v>1</v>
-      </c>
-      <c r="D32" s="75" t="s">
+      <c r="C32" s="74">
+        <v>1</v>
+      </c>
+      <c r="D32" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75">
+      <c r="E32" s="74"/>
+      <c r="F32" s="74">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="G32" s="75">
+      <c r="G32" s="74">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="H32" s="76" t="s">
+      <c r="H32" s="75" t="s">
         <v>285</v>
       </c>
-      <c r="I32" s="74" t="s">
+      <c r="I32" s="73" t="s">
         <v>82</v>
       </c>
       <c r="J32" s="24"/>
@@ -5879,27 +5879,27 @@
       </c>
     </row>
     <row r="33" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="73" t="s">
+      <c r="A33" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="74"/>
-      <c r="C33" s="75">
+      <c r="B33" s="73"/>
+      <c r="C33" s="74">
         <v>2</v>
       </c>
-      <c r="D33" s="75" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75">
+      <c r="D33" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
-      <c r="G33" s="75">
+      <c r="G33" s="74">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="H33" s="75"/>
-      <c r="I33" s="74" t="s">
+      <c r="H33" s="74"/>
+      <c r="I33" s="73" t="s">
         <v>83</v>
       </c>
       <c r="J33" s="24" t="s">
@@ -5935,10 +5935,10 @@
       <c r="J34" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="K34" s="77" t="s">
+      <c r="K34" s="80" t="s">
         <v>294</v>
       </c>
-      <c r="L34" s="77"/>
+      <c r="L34" s="80"/>
     </row>
     <row r="35" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="67" t="s">
@@ -5969,8 +5969,8 @@
       <c r="J35" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="K35" s="77"/>
-      <c r="L35" s="77"/>
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
     </row>
     <row r="36" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="67" t="s">
@@ -6001,8 +6001,8 @@
       <c r="J36" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="K36" s="77"/>
-      <c r="L36" s="77"/>
+      <c r="K36" s="80"/>
+      <c r="L36" s="80"/>
     </row>
     <row r="37" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="67" t="s">
@@ -6033,8 +6033,8 @@
       <c r="J37" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="K37" s="77"/>
-      <c r="L37" s="77"/>
+      <c r="K37" s="80"/>
+      <c r="L37" s="80"/>
     </row>
     <row r="38" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="67" t="s">
@@ -6065,8 +6065,8 @@
       <c r="J38" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="K38" s="77"/>
-      <c r="L38" s="77"/>
+      <c r="K38" s="80"/>
+      <c r="L38" s="80"/>
     </row>
     <row r="39" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="64" t="s">
@@ -6185,10 +6185,10 @@
       <c r="J42" s="24" t="s">
         <v>275</v>
       </c>
-      <c r="K42" s="77" t="s">
+      <c r="K42" s="80" t="s">
         <v>295</v>
       </c>
-      <c r="L42" s="77"/>
+      <c r="L42" s="80"/>
     </row>
     <row r="43" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="67" t="s">
@@ -6217,8 +6217,8 @@
       <c r="J43" s="24" t="s">
         <v>277</v>
       </c>
-      <c r="K43" s="77"/>
-      <c r="L43" s="77"/>
+      <c r="K43" s="80"/>
+      <c r="L43" s="80"/>
     </row>
     <row r="44" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="64" t="s">
@@ -6633,29 +6633,29 @@
       <c r="J57" s="24"/>
     </row>
     <row r="58" spans="1:10" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="78" t="s">
+      <c r="A58" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="B58" s="79"/>
-      <c r="C58" s="80">
+      <c r="B58" s="77"/>
+      <c r="C58" s="78">
         <v>12</v>
       </c>
-      <c r="D58" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="E58" s="80">
+      <c r="D58" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" s="78">
         <v>2</v>
       </c>
-      <c r="F58" s="80">
+      <c r="F58" s="78">
         <f t="shared" si="1"/>
         <v>195</v>
       </c>
-      <c r="G58" s="80">
+      <c r="G58" s="78">
         <f t="shared" si="2"/>
         <v>56</v>
       </c>
-      <c r="H58" s="80"/>
-      <c r="I58" s="79" t="s">
+      <c r="H58" s="78"/>
+      <c r="I58" s="77" t="s">
         <v>96</v>
       </c>
       <c r="J58" s="53"/>
@@ -7939,7 +7939,7 @@
   <dimension ref="A1:D314"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+      <selection activeCell="A44" sqref="A44:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9378,8 +9378,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A3:D197"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Añadido todo el codigo del estudio de SALARIO
</commit_message>
<xml_diff>
--- a/dr_EES_2018.xlsx
+++ b/dr_EES_2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a17ca3cd426fe78e/UOC Master/Tipología y Ciclo de vida de los datos/Práctica 2/PRA2/UOC-Tipologia-Practica2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_C15A127284F31E7D2FD47ADCFACCF11110496BC5" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{38A4D03B-1B48-4B70-B582-C9DD4125CBFE}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="11_C15A127284F31E7D2FD47ADCFACCF11110496BC5" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CE4AA41B-1EFB-4E9D-8391-EB370A7B4C29}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DiseñoParaExtraerColumnas" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="298">
   <si>
     <t>A</t>
   </si>
@@ -928,6 +928,12 @@
   </si>
   <si>
     <t>Revisar si hay outliers de 1 solo día de trabajo al mes o cosas así</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Puesto</t>
   </si>
 </sst>
 </file>
@@ -1754,9 +1760,9 @@
   </sheetPr>
   <dimension ref="A1:M1002"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:K21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I82" sqref="I82:J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3773,115 +3779,207 @@
       <c r="A82" s="10"/>
       <c r="B82" s="10"/>
       <c r="C82" s="10"/>
-      <c r="J82" s="10"/>
+      <c r="I82" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="J82" s="10" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="83" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="10"/>
       <c r="B83" s="10"/>
       <c r="C83" s="10"/>
-      <c r="J83" s="10"/>
+      <c r="I83" s="50">
+        <v>0</v>
+      </c>
+      <c r="J83" s="21" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="84" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="10"/>
       <c r="B84" s="10"/>
       <c r="C84" s="10"/>
-      <c r="J84" s="10"/>
+      <c r="I84" s="50">
+        <v>1</v>
+      </c>
+      <c r="J84" s="21" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="85" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="10"/>
       <c r="B85" s="10"/>
       <c r="C85" s="10"/>
-      <c r="J85" s="10"/>
+      <c r="I85" s="50">
+        <v>2</v>
+      </c>
+      <c r="J85" s="21" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="86" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="10"/>
       <c r="B86" s="10"/>
       <c r="C86" s="10"/>
-      <c r="J86" s="10"/>
+      <c r="I86" s="50">
+        <v>3</v>
+      </c>
+      <c r="J86" s="21" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="87" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A87" s="10"/>
       <c r="B87" s="10"/>
       <c r="C87" s="10"/>
       <c r="D87" s="31"/>
-      <c r="J87" s="10"/>
+      <c r="I87" s="50">
+        <v>4</v>
+      </c>
+      <c r="J87" s="21" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="88" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A88" s="10"/>
       <c r="B88" s="10"/>
       <c r="C88" s="10"/>
       <c r="D88" s="31"/>
-      <c r="J88" s="10"/>
+      <c r="I88" s="50">
+        <v>5</v>
+      </c>
+      <c r="J88" s="21" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="89" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A89" s="10"/>
       <c r="B89" s="10"/>
       <c r="C89" s="10"/>
       <c r="D89" s="31"/>
-      <c r="J89" s="10"/>
+      <c r="I89" s="50">
+        <v>6</v>
+      </c>
+      <c r="J89" s="21" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="90" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
       <c r="B90" s="10"/>
       <c r="C90" s="10"/>
       <c r="D90" s="31"/>
-      <c r="J90" s="10"/>
+      <c r="I90" s="50">
+        <v>7</v>
+      </c>
+      <c r="J90" s="21" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="91" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="8"/>
       <c r="C91" s="8"/>
+      <c r="I91" s="50">
+        <v>8</v>
+      </c>
+      <c r="J91" s="21" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="92" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="8"/>
       <c r="C92" s="8"/>
+      <c r="I92" s="50">
+        <v>9</v>
+      </c>
+      <c r="J92" s="21" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="93" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="14"/>
       <c r="B93" s="13"/>
       <c r="C93" s="14"/>
-      <c r="J93" s="13"/>
+      <c r="I93" s="50">
+        <v>10</v>
+      </c>
+      <c r="J93" s="21" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="94" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="10"/>
       <c r="B94" s="10"/>
       <c r="C94" s="10"/>
       <c r="D94" s="8"/>
-      <c r="J94" s="10"/>
+      <c r="I94" s="50">
+        <v>11</v>
+      </c>
+      <c r="J94" s="21" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="95" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="10"/>
       <c r="B95" s="10"/>
       <c r="C95" s="10"/>
       <c r="D95" s="8"/>
-      <c r="J95" s="10"/>
+      <c r="I95" s="50">
+        <v>12</v>
+      </c>
+      <c r="J95" s="21" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="96" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="10"/>
       <c r="B96" s="10"/>
       <c r="C96" s="10"/>
       <c r="D96" s="8"/>
-      <c r="J96" s="10"/>
+      <c r="I96" s="50">
+        <v>13</v>
+      </c>
+      <c r="J96" s="21" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="97" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="10"/>
       <c r="B97" s="10"/>
       <c r="C97" s="10"/>
       <c r="D97" s="8"/>
-      <c r="J97" s="10"/>
+      <c r="I97" s="50">
+        <v>14</v>
+      </c>
+      <c r="J97" s="21" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="98" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="10"/>
       <c r="B98" s="10"/>
       <c r="C98" s="10"/>
       <c r="D98" s="8"/>
-      <c r="J98" s="10"/>
+      <c r="I98" s="50">
+        <v>15</v>
+      </c>
+      <c r="J98" s="21" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="99" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="10"/>
       <c r="B99" s="10"/>
       <c r="C99" s="10"/>
       <c r="D99" s="8"/>
-      <c r="J99" s="10"/>
+      <c r="I99" s="50">
+        <v>16</v>
+      </c>
+      <c r="J99" s="21" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="100" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="10"/>
@@ -4934,9 +5032,9 @@
   </sheetPr>
   <dimension ref="A1:L1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I52" sqref="I52"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7938,7 +8036,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:D314"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="A44" sqref="A44:B46"/>
     </sheetView>
   </sheetViews>
@@ -9379,7 +9477,7 @@
   <dimension ref="A3:D197"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A47" sqref="A47:B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Añadidos textos hasta la comprobación de sueldos por nivel de estudios y sexo
</commit_message>
<xml_diff>
--- a/dr_EES_2018.xlsx
+++ b/dr_EES_2018.xlsx
@@ -4935,8 +4935,8 @@
   <dimension ref="A1:L1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I52" sqref="I52"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Añadidos textos hasta la compración de la predicción dependiendo del sexo
</commit_message>
<xml_diff>
--- a/dr_EES_2018.xlsx
+++ b/dr_EES_2018.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="39" documentId="11_C15A127284F31E7D2FD47ADCFACCF11110496BC5" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{38A4D03B-1B48-4B70-B582-C9DD4125CBFE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DiseñoParaExtraerColumnas" sheetId="4" r:id="rId1"/>
@@ -4934,8 +4934,8 @@
   </sheetPr>
   <dimension ref="A1:L1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -9378,8 +9378,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A3:D197"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>